<commit_message>
Update PLANILLA DE EVALUACIÓN FASE 1.xlsx
</commit_message>
<xml_diff>
--- a/Fase 1/Evidencias Grupales/PLANILLA DE EVALUACIÓN FASE 1.xlsx
+++ b/Fase 1/Evidencias Grupales/PLANILLA DE EVALUACIÓN FASE 1.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="99">
   <si>
     <t>INTEGRANTES</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>No logrado</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
   <si>
     <t>Puntaje</t>
@@ -834,7 +837,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -888,6 +891,9 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1308,7 +1314,7 @@
       </c>
       <c r="C4" s="8">
         <f>EVALUACION1!$C$24</f>
-        <v>7</v>
+        <v>6.1</v>
       </c>
       <c r="D4" s="8">
         <f>$C$35</f>
@@ -1316,7 +1322,7 @@
       </c>
       <c r="E4" s="9">
         <f t="shared" ref="E4:E6" si="1">C4*C$2+D4*D$2</f>
-        <v>7</v>
+        <v>6.325</v>
       </c>
       <c r="G4" s="10"/>
     </row>
@@ -1329,7 +1335,7 @@
       </c>
       <c r="C5" s="8">
         <f>EVALUACION1!$C$24</f>
-        <v>7</v>
+        <v>6.1</v>
       </c>
       <c r="D5" s="8">
         <f>C47</f>
@@ -1337,7 +1343,7 @@
       </c>
       <c r="E5" s="9">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6.325</v>
       </c>
       <c r="G5" s="10"/>
     </row>
@@ -1350,7 +1356,7 @@
       </c>
       <c r="C6" s="8">
         <f>EVALUACION1!$C$24</f>
-        <v>7</v>
+        <v>6.1</v>
       </c>
       <c r="D6" s="8">
         <f>C58</f>
@@ -1358,7 +1364,7 @@
       </c>
       <c r="E6" s="9">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6.325</v>
       </c>
       <c r="G6" s="10"/>
     </row>
@@ -1581,21 +1587,17 @@
       <c r="C17" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="21" t="str">
-        <f>IF($C17=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E17" s="21">
+      <c r="D17" s="21"/>
+      <c r="E17" s="21" t="str">
         <f t="shared" ref="E17:E18" si="6">IF(D17="X",100*0.1,"")</f>
-        <v>10</v>
-      </c>
-      <c r="F17" s="21" t="str">
-        <f>IF($C17=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G17" s="21" t="str">
+        <v/>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="21">
         <f t="shared" ref="G17:G18" si="7">IF(F17="X",60*0.1,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="H17" s="21" t="str">
         <f>IF($C17=ML,"X","")</f>
@@ -1623,21 +1625,17 @@
       <c r="C18" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="21" t="str">
-        <f>IF($C18=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E18" s="21">
+      <c r="D18" s="21"/>
+      <c r="E18" s="21" t="str">
         <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="F18" s="21" t="str">
-        <f>IF($C18=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G18" s="21" t="str">
+        <v/>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="21">
         <f t="shared" si="7"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="H18" s="21" t="str">
         <f>IF($C18=ML,"X","")</f>
@@ -1827,83 +1825,83 @@
     </row>
     <row r="23" ht="15.75" customHeight="1" outlineLevel="1">
       <c r="A23" s="17"/>
-      <c r="B23" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="23">
+      <c r="B23" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="24">
         <f>E23+G23+I23+K23</f>
-        <v>70</v>
-      </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24">
+        <v>62</v>
+      </c>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25">
         <f>SUM(E13:E22)</f>
-        <v>70</v>
-      </c>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24">
+        <v>50</v>
+      </c>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25">
         <f>SUM(G13:G22)</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24">
+        <v>12</v>
+      </c>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25">
         <f>SUM(I13:I22)</f>
         <v>0</v>
       </c>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24">
+      <c r="J23" s="25"/>
+      <c r="K23" s="25">
         <f>SUM(K13:K22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1" outlineLevel="1">
       <c r="A24" s="5"/>
-      <c r="B24" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="26">
+      <c r="B24" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="27">
         <f>VLOOKUP(C23,ESCALA_IEP!A2:B142,2,FALSE)</f>
-        <v>7</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1"/>
     <row r="26" ht="15.75" customHeight="1"/>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="28" t="s">
+      <c r="A27" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="29" t="str">
+      <c r="B27" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="30" t="str">
         <f>$B$4</f>
         <v>Alexander Eliot Lara Sepulveda</v>
       </c>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="32"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="17"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="34"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="35"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="17"/>
       <c r="B29" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>7</v>
@@ -1921,7 +1919,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="17"/>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="36" t="s">
         <v>9</v>
       </c>
       <c r="C30" s="5"/>
@@ -1934,7 +1932,7 @@
       </c>
       <c r="G30" s="16"/>
       <c r="H30" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I30" s="16"/>
       <c r="J30" s="14" t="s">
@@ -2070,90 +2068,90 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="17"/>
-      <c r="B34" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="37">
+      <c r="B34" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="38">
         <f>E34+G34+I34+K34</f>
         <v>30</v>
       </c>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24">
+      <c r="D34" s="25"/>
+      <c r="E34" s="25">
         <f>SUM(E31:E33)</f>
         <v>30</v>
       </c>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24">
+      <c r="F34" s="25"/>
+      <c r="G34" s="25">
         <f>SUM(G31:G33)</f>
         <v>0</v>
       </c>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24">
+      <c r="H34" s="25"/>
+      <c r="I34" s="25">
         <f>SUM(I31:I33)</f>
         <v>0</v>
       </c>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24">
+      <c r="J34" s="25"/>
+      <c r="K34" s="25">
         <f>SUM(K31:K33)</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="5"/>
-      <c r="B35" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="26">
+      <c r="B35" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="27">
         <f>VLOOKUP(C34,ESCALA_TRAB_EQUIP!A2:B62,2,FALSE)</f>
         <v>7</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="B36" s="39"/>
-      <c r="C36" s="40"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="41"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="B37" s="39"/>
-      <c r="C37" s="40"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="41"/>
     </row>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="28" t="s">
+      <c r="A39" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="29" t="str">
+      <c r="B39" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="30" t="str">
         <f>B5</f>
         <v>Franccesco Artuso Guliano Pacheco</v>
       </c>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="32"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="17"/>
       <c r="B40" s="5"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="33"/>
-      <c r="K40" s="34"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="34"/>
+      <c r="K40" s="35"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="17"/>
       <c r="B41" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>7</v>
@@ -2171,7 +2169,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="17"/>
-      <c r="B42" s="35" t="s">
+      <c r="B42" s="36" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="5"/>
@@ -2184,7 +2182,7 @@
       </c>
       <c r="G42" s="16"/>
       <c r="H42" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I42" s="16"/>
       <c r="J42" s="14" t="s">
@@ -2320,89 +2318,89 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="17"/>
-      <c r="B46" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46" s="37">
+      <c r="B46" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="38">
         <f>E46+G46+I46+K46</f>
         <v>30</v>
       </c>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24">
+      <c r="D46" s="25"/>
+      <c r="E46" s="25">
         <f>SUM(E43:E45)</f>
         <v>30</v>
       </c>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24">
+      <c r="F46" s="25"/>
+      <c r="G46" s="25">
         <f>SUM(G43:G45)</f>
         <v>0</v>
       </c>
-      <c r="H46" s="24"/>
-      <c r="I46" s="24">
+      <c r="H46" s="25"/>
+      <c r="I46" s="25">
         <f>SUM(I43:I45)</f>
         <v>0</v>
       </c>
-      <c r="J46" s="24"/>
-      <c r="K46" s="24">
+      <c r="J46" s="25"/>
+      <c r="K46" s="25">
         <f>SUM(K43:K45)</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="5"/>
-      <c r="B47" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C47" s="26">
+      <c r="B47" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="27">
         <f>VLOOKUP(C46,ESCALA_TRAB_EQUIP!A2:B62,2,FALSE)</f>
         <v>7</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="B48" s="39"/>
-      <c r="C48" s="40"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="41"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="B49" s="39"/>
-      <c r="C49" s="40"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="41"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B50" s="28" t="s">
+      <c r="A50" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C50" s="29" t="str">
+      <c r="B50" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" s="30" t="str">
         <f>B6</f>
         <v>Matias Ignacio Peñaloza Jara</v>
       </c>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="30"/>
-      <c r="G50" s="30"/>
-      <c r="H50" s="30"/>
-      <c r="I50" s="30"/>
-      <c r="J50" s="30"/>
-      <c r="K50" s="31"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
+      <c r="H50" s="31"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="31"/>
+      <c r="K50" s="32"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="17"/>
       <c r="B51" s="5"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="33"/>
-      <c r="H51" s="33"/>
-      <c r="I51" s="33"/>
-      <c r="J51" s="33"/>
-      <c r="K51" s="34"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="34"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="34"/>
+      <c r="G51" s="34"/>
+      <c r="H51" s="34"/>
+      <c r="I51" s="34"/>
+      <c r="J51" s="34"/>
+      <c r="K51" s="35"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="17"/>
       <c r="B52" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C52" s="13" t="s">
         <v>7</v>
@@ -2420,7 +2418,7 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="17"/>
-      <c r="B53" s="35" t="s">
+      <c r="B53" s="36" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="5"/>
@@ -2433,7 +2431,7 @@
       </c>
       <c r="G53" s="16"/>
       <c r="H53" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I53" s="16"/>
       <c r="J53" s="14" t="s">
@@ -2569,59 +2567,59 @@
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="17"/>
-      <c r="B57" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="C57" s="37">
+      <c r="B57" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57" s="38">
         <f>E57+G57+I57+K57</f>
         <v>30</v>
       </c>
-      <c r="D57" s="24">
+      <c r="D57" s="25">
         <f>COUNTIF(D55:D56,"X")</f>
         <v>2</v>
       </c>
-      <c r="E57" s="24">
+      <c r="E57" s="25">
         <f t="shared" ref="E57:K57" si="24">SUM(E54:E56)</f>
         <v>30</v>
       </c>
-      <c r="F57" s="24">
+      <c r="F57" s="25">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="G57" s="24">
+      <c r="G57" s="25">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="H57" s="24">
+      <c r="H57" s="25">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="I57" s="24">
+      <c r="I57" s="25">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="J57" s="24">
+      <c r="J57" s="25">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="K57" s="24">
+      <c r="K57" s="25">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="5"/>
-      <c r="B58" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C58" s="26">
+      <c r="B58" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" s="27">
         <f>VLOOKUP(C57,ESCALA_TRAB_EQUIP!A2:B62,2,FALSE)</f>
         <v>7</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="B59" s="39"/>
-      <c r="C59" s="40"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="41"/>
     </row>
     <row r="60" ht="15.75" customHeight="1"/>
     <row r="61" ht="15.75" customHeight="1"/>
@@ -3648,316 +3646,316 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="42" t="s">
+      <c r="A2" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="41" t="s">
+      <c r="B2" s="43" t="s">
         <v>23</v>
       </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="42" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="46" t="s">
+      <c r="A3" s="46"/>
+      <c r="B3" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="C3" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="D3" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="45"/>
+      <c r="F3" s="46"/>
     </row>
     <row r="4" ht="57.0" customHeight="1">
-      <c r="A4" s="49"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="50">
+      <c r="A4" s="50"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="51">
         <v>-0.3</v>
       </c>
-      <c r="E4" s="50">
+      <c r="E4" s="51">
         <v>0.0</v>
       </c>
-      <c r="F4" s="49"/>
+      <c r="F4" s="50"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="52" t="s">
+      <c r="A5" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="B5" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="C5" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="D5" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="53">
+      <c r="E5" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="54">
         <v>10.0</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="54" t="s">
+      <c r="A6" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="B6" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="C6" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="55" t="s">
+      <c r="D6" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="56">
+      <c r="E6" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="57">
         <v>5.0</v>
       </c>
     </row>
     <row r="7" ht="94.5" customHeight="1">
-      <c r="A7" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="57" t="s">
+      <c r="A7" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="B7" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="57" t="s">
+      <c r="C7" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="57" t="s">
+      <c r="D7" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="58">
+      <c r="E7" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="59">
         <v>10.0</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="57" t="s">
+      <c r="A8" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="57" t="s">
+      <c r="C8" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="D8" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="58">
+      <c r="E8" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="59">
         <v>5.0</v>
       </c>
     </row>
     <row r="9" ht="65.25" customHeight="1">
-      <c r="A9" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="52" t="s">
+      <c r="A9" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="B9" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="C9" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="52" t="s">
+      <c r="D9" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="53">
+      <c r="E9" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="54">
         <v>5.0</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="52" t="s">
+      <c r="A10" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="B10" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="C10" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="D10" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="53">
+      <c r="E10" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="54">
         <v>10.0</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="54" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="54" t="s">
+      <c r="A11" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="B11" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="C11" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="54" t="s">
+      <c r="D11" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="56">
+      <c r="E11" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="57">
         <v>10.0</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="59" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="55" t="s">
+      <c r="A12" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="B12" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="55" t="s">
+      <c r="C12" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="55" t="s">
+      <c r="D12" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="60">
+      <c r="E12" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="61">
         <v>5.0</v>
       </c>
     </row>
     <row r="13" ht="93.75" customHeight="1">
-      <c r="A13" s="57" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="57" t="s">
+      <c r="A13" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="B13" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="57" t="s">
+      <c r="C13" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="57" t="s">
+      <c r="D13" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="61">
+      <c r="E13" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="62">
         <v>5.0</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="57" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="57" t="s">
+      <c r="A14" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="57" t="s">
+      <c r="B14" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="57" t="s">
+      <c r="C14" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="57" t="s">
+      <c r="D14" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="61">
+      <c r="E14" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="62">
         <v>5.0</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="52" t="s">
+      <c r="A15" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="B15" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="52" t="s">
+      <c r="C15" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="D15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="F15" s="53">
+      <c r="E15" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="54">
         <v>10.0</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="B16" s="52" t="s">
+      <c r="A16" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="52" t="s">
+      <c r="B16" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="52" t="s">
+      <c r="C16" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="52" t="s">
+      <c r="D16" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="53">
+      <c r="E16" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="54">
         <v>10.0</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="51" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17" s="52" t="s">
+      <c r="A17" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="B17" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="52" t="s">
+      <c r="C17" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="E17" s="52" t="s">
+      <c r="D17" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="F17" s="53">
+      <c r="E17" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" s="54">
         <v>10.0</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="63">
+      <c r="A18" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="64">
         <v>1.0</v>
       </c>
     </row>
@@ -4973,1138 +4971,1138 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="64" t="s">
+      <c r="A1" s="65" t="s">
         <v>15</v>
       </c>
+      <c r="B1" s="65" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="64">
+      <c r="A2" s="65">
         <v>0.0</v>
       </c>
-      <c r="B2" s="65">
+      <c r="B2" s="66">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="64">
+      <c r="A3" s="65">
         <v>0.5</v>
       </c>
-      <c r="B3" s="65">
+      <c r="B3" s="66">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="64">
+      <c r="A4" s="65">
         <v>1.0</v>
       </c>
-      <c r="B4" s="65">
+      <c r="B4" s="66">
         <v>1.1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="64">
+      <c r="A5" s="65">
         <v>1.5</v>
       </c>
-      <c r="B5" s="65">
+      <c r="B5" s="66">
         <v>1.1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="64">
+      <c r="A6" s="65">
         <v>2.0</v>
       </c>
-      <c r="B6" s="65">
+      <c r="B6" s="66">
         <v>1.1</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="64">
+      <c r="A7" s="65">
         <v>2.5</v>
       </c>
-      <c r="B7" s="65">
+      <c r="B7" s="66">
         <v>1.2</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="64">
+      <c r="A8" s="65">
         <v>3.0</v>
       </c>
-      <c r="B8" s="65">
+      <c r="B8" s="66">
         <v>1.2</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="64">
+      <c r="A9" s="65">
         <v>3.5</v>
       </c>
-      <c r="B9" s="65">
+      <c r="B9" s="66">
         <v>1.3</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="64">
+      <c r="A10" s="65">
         <v>4.0</v>
       </c>
-      <c r="B10" s="65">
+      <c r="B10" s="66">
         <v>1.3</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="64">
+      <c r="A11" s="65">
         <v>4.5</v>
       </c>
-      <c r="B11" s="65">
+      <c r="B11" s="66">
         <v>1.3</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="64">
+      <c r="A12" s="65">
         <v>5.0</v>
       </c>
-      <c r="B12" s="65">
+      <c r="B12" s="66">
         <v>1.4</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="64">
+      <c r="A13" s="65">
         <v>5.5</v>
       </c>
-      <c r="B13" s="65">
+      <c r="B13" s="66">
         <v>1.4</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="64">
+      <c r="A14" s="65">
         <v>6.0</v>
       </c>
-      <c r="B14" s="65">
+      <c r="B14" s="66">
         <v>1.4</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="64">
+      <c r="A15" s="65">
         <v>6.5</v>
       </c>
-      <c r="B15" s="65">
+      <c r="B15" s="66">
         <v>1.5</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="64">
+      <c r="A16" s="65">
         <v>7.0</v>
       </c>
-      <c r="B16" s="65">
+      <c r="B16" s="66">
         <v>1.5</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="64">
+      <c r="A17" s="65">
         <v>7.5</v>
       </c>
-      <c r="B17" s="65">
+      <c r="B17" s="66">
         <v>1.5</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="64">
+      <c r="A18" s="65">
         <v>8.0</v>
       </c>
-      <c r="B18" s="65">
+      <c r="B18" s="66">
         <v>1.6</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="64">
+      <c r="A19" s="65">
         <v>8.5</v>
       </c>
-      <c r="B19" s="65">
+      <c r="B19" s="66">
         <v>1.6</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="64">
+      <c r="A20" s="65">
         <v>9.0</v>
       </c>
-      <c r="B20" s="65">
+      <c r="B20" s="66">
         <v>1.6</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="64">
+      <c r="A21" s="65">
         <v>9.5</v>
       </c>
-      <c r="B21" s="65">
+      <c r="B21" s="66">
         <v>1.7</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="64">
+      <c r="A22" s="65">
         <v>10.0</v>
       </c>
-      <c r="B22" s="65">
+      <c r="B22" s="66">
         <v>1.7</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="64">
+      <c r="A23" s="65">
         <v>10.5</v>
       </c>
-      <c r="B23" s="65">
+      <c r="B23" s="66">
         <v>1.8</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="64">
+      <c r="A24" s="65">
         <v>11.0</v>
       </c>
-      <c r="B24" s="65">
+      <c r="B24" s="66">
         <v>1.8</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="64">
+      <c r="A25" s="65">
         <v>11.5</v>
       </c>
-      <c r="B25" s="65">
+      <c r="B25" s="66">
         <v>1.8</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="64">
+      <c r="A26" s="65">
         <v>12.0</v>
       </c>
-      <c r="B26" s="65">
+      <c r="B26" s="66">
         <v>1.9</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="64">
+      <c r="A27" s="65">
         <v>12.5</v>
       </c>
-      <c r="B27" s="65">
+      <c r="B27" s="66">
         <v>1.9</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="64">
+      <c r="A28" s="65">
         <v>13.0</v>
       </c>
-      <c r="B28" s="65">
+      <c r="B28" s="66">
         <v>1.9</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="64">
+      <c r="A29" s="65">
         <v>13.5</v>
       </c>
-      <c r="B29" s="65">
+      <c r="B29" s="66">
         <v>2.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="64">
+      <c r="A30" s="65">
         <v>14.0</v>
       </c>
-      <c r="B30" s="65">
+      <c r="B30" s="66">
         <v>2.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="64">
+      <c r="A31" s="65">
         <v>14.5</v>
       </c>
-      <c r="B31" s="65">
+      <c r="B31" s="66">
         <v>2.0</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="64">
+      <c r="A32" s="65">
         <v>15.0</v>
       </c>
-      <c r="B32" s="65">
+      <c r="B32" s="66">
         <v>2.1</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="64">
+      <c r="A33" s="65">
         <v>15.5</v>
       </c>
-      <c r="B33" s="65">
+      <c r="B33" s="66">
         <v>2.1</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="64">
+      <c r="A34" s="65">
         <v>16.0</v>
       </c>
-      <c r="B34" s="65">
+      <c r="B34" s="66">
         <v>2.1</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="64">
+      <c r="A35" s="65">
         <v>16.5</v>
       </c>
-      <c r="B35" s="65">
+      <c r="B35" s="66">
         <v>2.2</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="64">
+      <c r="A36" s="65">
         <v>17.0</v>
       </c>
-      <c r="B36" s="65">
+      <c r="B36" s="66">
         <v>2.2</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="64">
+      <c r="A37" s="65">
         <v>17.5</v>
       </c>
-      <c r="B37" s="65">
+      <c r="B37" s="66">
         <v>2.3</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="64">
+      <c r="A38" s="65">
         <v>18.0</v>
       </c>
-      <c r="B38" s="65">
+      <c r="B38" s="66">
         <v>2.3</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="64">
+      <c r="A39" s="65">
         <v>18.5</v>
       </c>
-      <c r="B39" s="65">
+      <c r="B39" s="66">
         <v>2.3</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="64">
+      <c r="A40" s="65">
         <v>19.0</v>
       </c>
-      <c r="B40" s="65">
+      <c r="B40" s="66">
         <v>2.4</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="64">
+      <c r="A41" s="65">
         <v>19.5</v>
       </c>
-      <c r="B41" s="65">
+      <c r="B41" s="66">
         <v>2.4</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="64">
+      <c r="A42" s="65">
         <v>20.0</v>
       </c>
-      <c r="B42" s="65">
+      <c r="B42" s="66">
         <v>2.4</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="64">
+      <c r="A43" s="65">
         <v>20.5</v>
       </c>
-      <c r="B43" s="65">
+      <c r="B43" s="66">
         <v>2.5</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="64">
+      <c r="A44" s="65">
         <v>21.0</v>
       </c>
-      <c r="B44" s="65">
+      <c r="B44" s="66">
         <v>2.5</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="64">
+      <c r="A45" s="65">
         <v>21.5</v>
       </c>
-      <c r="B45" s="65">
+      <c r="B45" s="66">
         <v>2.5</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="64">
+      <c r="A46" s="65">
         <v>22.0</v>
       </c>
-      <c r="B46" s="65">
+      <c r="B46" s="66">
         <v>2.6</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="64">
+      <c r="A47" s="65">
         <v>22.5</v>
       </c>
-      <c r="B47" s="65">
+      <c r="B47" s="66">
         <v>2.6</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="64">
+      <c r="A48" s="65">
         <v>23.0</v>
       </c>
-      <c r="B48" s="65">
+      <c r="B48" s="66">
         <v>2.6</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="64">
+      <c r="A49" s="65">
         <v>23.5</v>
       </c>
-      <c r="B49" s="65">
+      <c r="B49" s="66">
         <v>2.7</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="64">
+      <c r="A50" s="65">
         <v>24.0</v>
       </c>
-      <c r="B50" s="65">
+      <c r="B50" s="66">
         <v>2.7</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="64">
+      <c r="A51" s="65">
         <v>24.5</v>
       </c>
-      <c r="B51" s="65">
+      <c r="B51" s="66">
         <v>2.8</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="64">
+      <c r="A52" s="65">
         <v>25.0</v>
       </c>
-      <c r="B52" s="65">
+      <c r="B52" s="66">
         <v>2.8</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="64">
+      <c r="A53" s="65">
         <v>25.5</v>
       </c>
-      <c r="B53" s="65">
+      <c r="B53" s="66">
         <v>2.8</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="64">
+      <c r="A54" s="65">
         <v>26.0</v>
       </c>
-      <c r="B54" s="65">
+      <c r="B54" s="66">
         <v>2.9</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="64">
+      <c r="A55" s="65">
         <v>26.5</v>
       </c>
-      <c r="B55" s="65">
+      <c r="B55" s="66">
         <v>2.9</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="64">
+      <c r="A56" s="65">
         <v>27.0</v>
       </c>
-      <c r="B56" s="65">
+      <c r="B56" s="66">
         <v>2.9</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="64">
+      <c r="A57" s="65">
         <v>27.5</v>
       </c>
-      <c r="B57" s="65">
+      <c r="B57" s="66">
         <v>3.0</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="64">
+      <c r="A58" s="65">
         <v>28.0</v>
       </c>
-      <c r="B58" s="65">
+      <c r="B58" s="66">
         <v>3.0</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="64">
+      <c r="A59" s="65">
         <v>28.5</v>
       </c>
-      <c r="B59" s="65">
+      <c r="B59" s="66">
         <v>3.0</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="64">
+      <c r="A60" s="65">
         <v>29.0</v>
       </c>
-      <c r="B60" s="65">
+      <c r="B60" s="66">
         <v>3.1</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="64">
+      <c r="A61" s="65">
         <v>29.5</v>
       </c>
-      <c r="B61" s="65">
+      <c r="B61" s="66">
         <v>3.1</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="64">
+      <c r="A62" s="65">
         <v>30.0</v>
       </c>
-      <c r="B62" s="65">
+      <c r="B62" s="66">
         <v>3.1</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="64">
+      <c r="A63" s="65">
         <v>30.5</v>
       </c>
-      <c r="B63" s="65">
+      <c r="B63" s="66">
         <v>3.2</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="64">
+      <c r="A64" s="65">
         <v>31.0</v>
       </c>
-      <c r="B64" s="65">
+      <c r="B64" s="66">
         <v>3.2</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="64">
+      <c r="A65" s="65">
         <v>31.5</v>
       </c>
-      <c r="B65" s="65">
+      <c r="B65" s="66">
         <v>3.3</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="64">
+      <c r="A66" s="65">
         <v>32.0</v>
       </c>
-      <c r="B66" s="65">
+      <c r="B66" s="66">
         <v>3.3</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="64">
+      <c r="A67" s="65">
         <v>32.5</v>
       </c>
-      <c r="B67" s="65">
+      <c r="B67" s="66">
         <v>3.3</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="64">
+      <c r="A68" s="65">
         <v>33.0</v>
       </c>
-      <c r="B68" s="65">
+      <c r="B68" s="66">
         <v>3.4</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="64">
+      <c r="A69" s="65">
         <v>33.5</v>
       </c>
-      <c r="B69" s="65">
+      <c r="B69" s="66">
         <v>3.4</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="64">
+      <c r="A70" s="65">
         <v>34.0</v>
       </c>
-      <c r="B70" s="65">
+      <c r="B70" s="66">
         <v>3.4</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="64">
+      <c r="A71" s="65">
         <v>34.5</v>
       </c>
-      <c r="B71" s="65">
+      <c r="B71" s="66">
         <v>3.5</v>
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="64">
+      <c r="A72" s="65">
         <v>35.0</v>
       </c>
-      <c r="B72" s="65">
+      <c r="B72" s="66">
         <v>3.5</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="64">
+      <c r="A73" s="65">
         <v>35.5</v>
       </c>
-      <c r="B73" s="65">
+      <c r="B73" s="66">
         <v>3.5</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="64">
+      <c r="A74" s="65">
         <v>36.0</v>
       </c>
-      <c r="B74" s="65">
+      <c r="B74" s="66">
         <v>3.6</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="64">
+      <c r="A75" s="65">
         <v>36.5</v>
       </c>
-      <c r="B75" s="65">
+      <c r="B75" s="66">
         <v>3.6</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="64">
+      <c r="A76" s="65">
         <v>37.0</v>
       </c>
-      <c r="B76" s="65">
+      <c r="B76" s="66">
         <v>3.6</v>
       </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="64">
+      <c r="A77" s="65">
         <v>37.5</v>
       </c>
-      <c r="B77" s="65">
+      <c r="B77" s="66">
         <v>3.7</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="64">
+      <c r="A78" s="65">
         <v>38.0</v>
       </c>
-      <c r="B78" s="65">
+      <c r="B78" s="66">
         <v>3.7</v>
       </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="64">
+      <c r="A79" s="65">
         <v>38.5</v>
       </c>
-      <c r="B79" s="65">
+      <c r="B79" s="66">
         <v>3.8</v>
       </c>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="64">
+      <c r="A80" s="65">
         <v>39.0</v>
       </c>
-      <c r="B80" s="65">
+      <c r="B80" s="66">
         <v>3.8</v>
       </c>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="64">
+      <c r="A81" s="65">
         <v>39.5</v>
       </c>
-      <c r="B81" s="65">
+      <c r="B81" s="66">
         <v>3.8</v>
       </c>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="64">
+      <c r="A82" s="65">
         <v>40.0</v>
       </c>
-      <c r="B82" s="65">
+      <c r="B82" s="66">
         <v>3.9</v>
       </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="64">
+      <c r="A83" s="65">
         <v>40.5</v>
       </c>
-      <c r="B83" s="65">
+      <c r="B83" s="66">
         <v>3.9</v>
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="64">
+      <c r="A84" s="65">
         <v>41.0</v>
       </c>
-      <c r="B84" s="65">
+      <c r="B84" s="66">
         <v>3.9</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="64">
+      <c r="A85" s="65">
         <v>41.5</v>
       </c>
-      <c r="B85" s="65">
+      <c r="B85" s="66">
         <v>4.0</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="64">
+      <c r="A86" s="65">
         <v>42.0</v>
       </c>
-      <c r="B86" s="65">
+      <c r="B86" s="66">
         <v>4.0</v>
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="64">
+      <c r="A87" s="65">
         <v>42.5</v>
       </c>
-      <c r="B87" s="65">
+      <c r="B87" s="66">
         <v>4.1</v>
       </c>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="64">
+      <c r="A88" s="65">
         <v>43.0</v>
       </c>
-      <c r="B88" s="65">
+      <c r="B88" s="66">
         <v>4.1</v>
       </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="64">
+      <c r="A89" s="65">
         <v>43.5</v>
       </c>
-      <c r="B89" s="65">
+      <c r="B89" s="66">
         <v>4.2</v>
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="64">
+      <c r="A90" s="65">
         <v>44.0</v>
       </c>
-      <c r="B90" s="65">
+      <c r="B90" s="66">
         <v>4.2</v>
       </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="64">
+      <c r="A91" s="65">
         <v>44.5</v>
       </c>
-      <c r="B91" s="65">
+      <c r="B91" s="66">
         <v>4.3</v>
       </c>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="64">
+      <c r="A92" s="65">
         <v>45.0</v>
       </c>
-      <c r="B92" s="65">
+      <c r="B92" s="66">
         <v>4.3</v>
       </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="64">
+      <c r="A93" s="65">
         <v>45.5</v>
       </c>
-      <c r="B93" s="65">
+      <c r="B93" s="66">
         <v>4.4</v>
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="64">
+      <c r="A94" s="65">
         <v>46.0</v>
       </c>
-      <c r="B94" s="65">
+      <c r="B94" s="66">
         <v>4.4</v>
       </c>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="64">
+      <c r="A95" s="65">
         <v>46.5</v>
       </c>
-      <c r="B95" s="65">
+      <c r="B95" s="66">
         <v>4.5</v>
       </c>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="64">
+      <c r="A96" s="65">
         <v>47.0</v>
       </c>
-      <c r="B96" s="65">
+      <c r="B96" s="66">
         <v>4.5</v>
       </c>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="64">
+      <c r="A97" s="65">
         <v>47.5</v>
       </c>
-      <c r="B97" s="65">
+      <c r="B97" s="66">
         <v>4.6</v>
       </c>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="64">
+      <c r="A98" s="65">
         <v>48.0</v>
       </c>
-      <c r="B98" s="65">
+      <c r="B98" s="66">
         <v>4.6</v>
       </c>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="64">
+      <c r="A99" s="65">
         <v>48.5</v>
       </c>
-      <c r="B99" s="65">
+      <c r="B99" s="66">
         <v>4.7</v>
       </c>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="64">
+      <c r="A100" s="65">
         <v>49.0</v>
       </c>
-      <c r="B100" s="65">
+      <c r="B100" s="66">
         <v>4.8</v>
       </c>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="64">
+      <c r="A101" s="65">
         <v>49.5</v>
       </c>
-      <c r="B101" s="65">
+      <c r="B101" s="66">
         <v>4.8</v>
       </c>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="64">
+      <c r="A102" s="65">
         <v>50.0</v>
       </c>
-      <c r="B102" s="65">
+      <c r="B102" s="66">
         <v>4.9</v>
       </c>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="64">
+      <c r="A103" s="65">
         <v>50.5</v>
       </c>
-      <c r="B103" s="65">
+      <c r="B103" s="66">
         <v>4.9</v>
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="64">
+      <c r="A104" s="65">
         <v>51.0</v>
       </c>
-      <c r="B104" s="65">
+      <c r="B104" s="66">
         <v>5.0</v>
       </c>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="64">
+      <c r="A105" s="65">
         <v>51.5</v>
       </c>
-      <c r="B105" s="65">
+      <c r="B105" s="66">
         <v>5.0</v>
       </c>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="64">
+      <c r="A106" s="65">
         <v>52.0</v>
       </c>
-      <c r="B106" s="65">
+      <c r="B106" s="66">
         <v>5.1</v>
       </c>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="64">
+      <c r="A107" s="65">
         <v>52.5</v>
       </c>
-      <c r="B107" s="65">
+      <c r="B107" s="66">
         <v>5.1</v>
       </c>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="64">
+      <c r="A108" s="65">
         <v>53.0</v>
       </c>
-      <c r="B108" s="65">
+      <c r="B108" s="66">
         <v>5.2</v>
       </c>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="64">
+      <c r="A109" s="65">
         <v>53.5</v>
       </c>
-      <c r="B109" s="65">
+      <c r="B109" s="66">
         <v>5.2</v>
       </c>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="64">
+      <c r="A110" s="65">
         <v>54.0</v>
       </c>
-      <c r="B110" s="65">
+      <c r="B110" s="66">
         <v>5.3</v>
       </c>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="64">
+      <c r="A111" s="65">
         <v>54.5</v>
       </c>
-      <c r="B111" s="65">
+      <c r="B111" s="66">
         <v>5.3</v>
       </c>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="64">
+      <c r="A112" s="65">
         <v>55.0</v>
       </c>
-      <c r="B112" s="65">
+      <c r="B112" s="66">
         <v>5.4</v>
       </c>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="64">
+      <c r="A113" s="65">
         <v>55.5</v>
       </c>
-      <c r="B113" s="65">
+      <c r="B113" s="66">
         <v>5.4</v>
       </c>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="64">
+      <c r="A114" s="65">
         <v>56.0</v>
       </c>
-      <c r="B114" s="65">
+      <c r="B114" s="66">
         <v>5.5</v>
       </c>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="64">
+      <c r="A115" s="65">
         <v>56.5</v>
       </c>
-      <c r="B115" s="65">
+      <c r="B115" s="66">
         <v>5.6</v>
       </c>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="64">
+      <c r="A116" s="65">
         <v>57.0</v>
       </c>
-      <c r="B116" s="65">
+      <c r="B116" s="66">
         <v>5.6</v>
       </c>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="64">
+      <c r="A117" s="65">
         <v>57.5</v>
       </c>
-      <c r="B117" s="65">
+      <c r="B117" s="66">
         <v>5.7</v>
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="64">
+      <c r="A118" s="65">
         <v>58.0</v>
       </c>
-      <c r="B118" s="65">
+      <c r="B118" s="66">
         <v>5.7</v>
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="64">
+      <c r="A119" s="65">
         <v>58.5</v>
       </c>
-      <c r="B119" s="65">
+      <c r="B119" s="66">
         <v>5.8</v>
       </c>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="64">
+      <c r="A120" s="65">
         <v>59.0</v>
       </c>
-      <c r="B120" s="65">
+      <c r="B120" s="66">
         <v>5.8</v>
       </c>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="64">
+      <c r="A121" s="65">
         <v>59.5</v>
       </c>
-      <c r="B121" s="65">
+      <c r="B121" s="66">
         <v>5.9</v>
       </c>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="64">
+      <c r="A122" s="65">
         <v>60.0</v>
       </c>
-      <c r="B122" s="65">
+      <c r="B122" s="66">
         <v>5.9</v>
       </c>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="64">
+      <c r="A123" s="65">
         <v>60.5</v>
       </c>
-      <c r="B123" s="65">
+      <c r="B123" s="66">
         <v>6.0</v>
       </c>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="64">
+      <c r="A124" s="65">
         <v>61.0</v>
       </c>
-      <c r="B124" s="65">
+      <c r="B124" s="66">
         <v>6.0</v>
       </c>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="64">
+      <c r="A125" s="65">
         <v>61.5</v>
       </c>
-      <c r="B125" s="65">
+      <c r="B125" s="66">
         <v>6.1</v>
       </c>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="64">
+      <c r="A126" s="65">
         <v>62.0</v>
       </c>
-      <c r="B126" s="65">
+      <c r="B126" s="66">
         <v>6.1</v>
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="64">
+      <c r="A127" s="65">
         <v>62.5</v>
       </c>
-      <c r="B127" s="65">
+      <c r="B127" s="66">
         <v>6.2</v>
       </c>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="64">
+      <c r="A128" s="65">
         <v>63.0</v>
       </c>
-      <c r="B128" s="65">
+      <c r="B128" s="66">
         <v>6.3</v>
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="64">
+      <c r="A129" s="65">
         <v>63.5</v>
       </c>
-      <c r="B129" s="65">
+      <c r="B129" s="66">
         <v>6.3</v>
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="64">
+      <c r="A130" s="65">
         <v>64.0</v>
       </c>
-      <c r="B130" s="65">
+      <c r="B130" s="66">
         <v>6.4</v>
       </c>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="64">
+      <c r="A131" s="65">
         <v>64.5</v>
       </c>
-      <c r="B131" s="65">
+      <c r="B131" s="66">
         <v>6.4</v>
       </c>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="64">
+      <c r="A132" s="65">
         <v>65.0</v>
       </c>
-      <c r="B132" s="65">
+      <c r="B132" s="66">
         <v>6.5</v>
       </c>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="64">
+      <c r="A133" s="65">
         <v>65.5</v>
       </c>
-      <c r="B133" s="65">
+      <c r="B133" s="66">
         <v>6.5</v>
       </c>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="64">
+      <c r="A134" s="65">
         <v>66.0</v>
       </c>
-      <c r="B134" s="65">
+      <c r="B134" s="66">
         <v>6.6</v>
       </c>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="64">
+      <c r="A135" s="65">
         <v>66.5</v>
       </c>
-      <c r="B135" s="65">
+      <c r="B135" s="66">
         <v>6.6</v>
       </c>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="64">
+      <c r="A136" s="65">
         <v>67.0</v>
       </c>
-      <c r="B136" s="65">
+      <c r="B136" s="66">
         <v>6.7</v>
       </c>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="64">
+      <c r="A137" s="65">
         <v>67.5</v>
       </c>
-      <c r="B137" s="65">
+      <c r="B137" s="66">
         <v>6.7</v>
       </c>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="64">
+      <c r="A138" s="65">
         <v>68.0</v>
       </c>
-      <c r="B138" s="65">
+      <c r="B138" s="66">
         <v>6.8</v>
       </c>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="64">
+      <c r="A139" s="65">
         <v>68.5</v>
       </c>
-      <c r="B139" s="65">
+      <c r="B139" s="66">
         <v>6.8</v>
       </c>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="64">
+      <c r="A140" s="65">
         <v>69.0</v>
       </c>
-      <c r="B140" s="65">
+      <c r="B140" s="66">
         <v>6.9</v>
       </c>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="64">
+      <c r="A141" s="65">
         <v>69.5</v>
       </c>
-      <c r="B141" s="65">
+      <c r="B141" s="66">
         <v>6.9</v>
       </c>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="64">
+      <c r="A142" s="65">
         <v>70.0</v>
       </c>
-      <c r="B142" s="65">
+      <c r="B142" s="66">
         <v>7.0</v>
       </c>
     </row>
@@ -6988,15 +6986,15 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="64" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="64" t="s">
+      <c r="A1" s="65" t="s">
         <v>94</v>
       </c>
+      <c r="B1" s="65" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="64">
+      <c r="A2" s="65">
         <v>0.0</v>
       </c>
       <c r="B2" s="10">
@@ -7004,7 +7002,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="64">
+      <c r="A3" s="65">
         <v>1.0</v>
       </c>
       <c r="B3" s="10">
@@ -7012,7 +7010,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="64">
+      <c r="A4" s="65">
         <v>2.0</v>
       </c>
       <c r="B4" s="10">
@@ -7020,7 +7018,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="64">
+      <c r="A5" s="65">
         <v>3.0</v>
       </c>
       <c r="B5" s="10">
@@ -7028,7 +7026,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="64">
+      <c r="A6" s="65">
         <v>4.0</v>
       </c>
       <c r="B6" s="10">
@@ -7036,7 +7034,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="64">
+      <c r="A7" s="65">
         <v>5.0</v>
       </c>
       <c r="B7" s="10">
@@ -7044,7 +7042,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="64">
+      <c r="A8" s="65">
         <v>6.0</v>
       </c>
       <c r="B8" s="10">
@@ -7052,7 +7050,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="64">
+      <c r="A9" s="65">
         <v>7.0</v>
       </c>
       <c r="B9" s="10">
@@ -7060,7 +7058,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="64">
+      <c r="A10" s="65">
         <v>8.0</v>
       </c>
       <c r="B10" s="10">
@@ -7068,7 +7066,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="64">
+      <c r="A11" s="65">
         <v>9.0</v>
       </c>
       <c r="B11" s="10">
@@ -7076,7 +7074,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="64">
+      <c r="A12" s="65">
         <v>10.0</v>
       </c>
       <c r="B12" s="10">
@@ -7084,7 +7082,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="64">
+      <c r="A13" s="65">
         <v>11.0</v>
       </c>
       <c r="B13" s="10">
@@ -7092,7 +7090,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="64">
+      <c r="A14" s="65">
         <v>12.0</v>
       </c>
       <c r="B14" s="10">
@@ -7100,7 +7098,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="64">
+      <c r="A15" s="65">
         <v>13.0</v>
       </c>
       <c r="B15" s="10">
@@ -7108,7 +7106,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="64">
+      <c r="A16" s="65">
         <v>14.0</v>
       </c>
       <c r="B16" s="10">
@@ -7116,7 +7114,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="64">
+      <c r="A17" s="65">
         <v>15.0</v>
       </c>
       <c r="B17" s="10">
@@ -7124,7 +7122,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="64">
+      <c r="A18" s="65">
         <v>16.0</v>
       </c>
       <c r="B18" s="10">
@@ -7132,7 +7130,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="64">
+      <c r="A19" s="65">
         <v>17.0</v>
       </c>
       <c r="B19" s="10">
@@ -7140,7 +7138,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="64">
+      <c r="A20" s="65">
         <v>18.0</v>
       </c>
       <c r="B20" s="10">
@@ -7148,7 +7146,7 @@
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="64">
+      <c r="A21" s="65">
         <v>19.0</v>
       </c>
       <c r="B21" s="10">
@@ -7156,7 +7154,7 @@
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="64">
+      <c r="A22" s="65">
         <v>20.0</v>
       </c>
       <c r="B22" s="10">
@@ -7164,7 +7162,7 @@
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="64">
+      <c r="A23" s="65">
         <v>21.0</v>
       </c>
       <c r="B23" s="10">
@@ -7172,7 +7170,7 @@
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="64">
+      <c r="A24" s="65">
         <v>22.0</v>
       </c>
       <c r="B24" s="10">
@@ -7180,7 +7178,7 @@
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="64">
+      <c r="A25" s="65">
         <v>23.0</v>
       </c>
       <c r="B25" s="10">
@@ -7188,7 +7186,7 @@
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="64">
+      <c r="A26" s="65">
         <v>24.0</v>
       </c>
       <c r="B26" s="10">
@@ -7196,7 +7194,7 @@
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="64">
+      <c r="A27" s="65">
         <v>25.0</v>
       </c>
       <c r="B27" s="10">
@@ -7204,7 +7202,7 @@
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="64">
+      <c r="A28" s="65">
         <v>26.0</v>
       </c>
       <c r="B28" s="10">
@@ -7212,7 +7210,7 @@
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="64">
+      <c r="A29" s="65">
         <v>27.0</v>
       </c>
       <c r="B29" s="10">
@@ -7220,7 +7218,7 @@
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="64">
+      <c r="A30" s="65">
         <v>28.0</v>
       </c>
       <c r="B30" s="10">
@@ -7228,7 +7226,7 @@
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="64">
+      <c r="A31" s="65">
         <v>29.0</v>
       </c>
       <c r="B31" s="10">
@@ -7236,7 +7234,7 @@
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="64">
+      <c r="A32" s="65">
         <v>30.0</v>
       </c>
       <c r="B32" s="10">
@@ -7244,7 +7242,7 @@
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="64">
+      <c r="A33" s="65">
         <v>31.0</v>
       </c>
       <c r="B33" s="10">
@@ -7252,7 +7250,7 @@
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="64">
+      <c r="A34" s="65">
         <v>32.0</v>
       </c>
       <c r="B34" s="10">
@@ -7260,7 +7258,7 @@
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="64">
+      <c r="A35" s="65">
         <v>33.0</v>
       </c>
       <c r="B35" s="10">
@@ -7268,7 +7266,7 @@
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="64">
+      <c r="A36" s="65">
         <v>34.0</v>
       </c>
       <c r="B36" s="10">
@@ -7276,7 +7274,7 @@
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="64">
+      <c r="A37" s="65">
         <v>35.0</v>
       </c>
       <c r="B37" s="10">
@@ -7284,7 +7282,7 @@
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="64">
+      <c r="A38" s="65">
         <v>36.0</v>
       </c>
       <c r="B38" s="10">
@@ -7292,7 +7290,7 @@
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="64">
+      <c r="A39" s="65">
         <v>37.0</v>
       </c>
       <c r="B39" s="10">
@@ -7300,7 +7298,7 @@
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="64">
+      <c r="A40" s="65">
         <v>38.0</v>
       </c>
       <c r="B40" s="10">
@@ -7308,7 +7306,7 @@
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="64">
+      <c r="A41" s="65">
         <v>39.0</v>
       </c>
       <c r="B41" s="10">
@@ -7316,7 +7314,7 @@
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="64">
+      <c r="A42" s="65">
         <v>40.0</v>
       </c>
       <c r="B42" s="10">
@@ -7324,7 +7322,7 @@
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="64">
+      <c r="A43" s="65">
         <v>41.0</v>
       </c>
       <c r="B43" s="10">
@@ -7332,7 +7330,7 @@
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="64">
+      <c r="A44" s="65">
         <v>42.0</v>
       </c>
       <c r="B44" s="10">
@@ -7340,7 +7338,7 @@
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="64">
+      <c r="A45" s="65">
         <v>43.0</v>
       </c>
       <c r="B45" s="10">
@@ -7348,7 +7346,7 @@
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="64">
+      <c r="A46" s="65">
         <v>44.0</v>
       </c>
       <c r="B46" s="10">
@@ -7356,7 +7354,7 @@
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="64">
+      <c r="A47" s="65">
         <v>45.0</v>
       </c>
       <c r="B47" s="10">
@@ -7364,7 +7362,7 @@
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="64">
+      <c r="A48" s="65">
         <v>46.0</v>
       </c>
       <c r="B48" s="10">
@@ -7372,7 +7370,7 @@
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="64">
+      <c r="A49" s="65">
         <v>47.0</v>
       </c>
       <c r="B49" s="10">
@@ -7380,7 +7378,7 @@
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="64">
+      <c r="A50" s="65">
         <v>48.0</v>
       </c>
       <c r="B50" s="10">
@@ -7388,7 +7386,7 @@
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="64">
+      <c r="A51" s="65">
         <v>49.0</v>
       </c>
       <c r="B51" s="10">
@@ -7396,7 +7394,7 @@
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="64">
+      <c r="A52" s="65">
         <v>50.0</v>
       </c>
       <c r="B52" s="10">
@@ -7404,7 +7402,7 @@
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="64">
+      <c r="A53" s="65">
         <v>51.0</v>
       </c>
       <c r="B53" s="10">
@@ -7412,7 +7410,7 @@
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="64">
+      <c r="A54" s="65">
         <v>52.0</v>
       </c>
       <c r="B54" s="10">
@@ -8387,498 +8385,498 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="64" t="s">
+      <c r="A1" s="65" t="s">
         <v>15</v>
       </c>
+      <c r="B1" s="65" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="64">
+      <c r="A2" s="65">
         <v>0.0</v>
       </c>
-      <c r="B2" s="65">
+      <c r="B2" s="66">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="64">
+      <c r="A3" s="65">
         <v>0.5</v>
       </c>
-      <c r="B3" s="65">
+      <c r="B3" s="66">
         <v>1.1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="64">
+      <c r="A4" s="65">
         <v>1.0</v>
       </c>
-      <c r="B4" s="65">
+      <c r="B4" s="66">
         <v>1.2</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="64">
+      <c r="A5" s="65">
         <v>1.5</v>
       </c>
-      <c r="B5" s="65">
+      <c r="B5" s="66">
         <v>1.3</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="64">
+      <c r="A6" s="65">
         <v>2.0</v>
       </c>
-      <c r="B6" s="65">
+      <c r="B6" s="66">
         <v>1.3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="64">
+      <c r="A7" s="65">
         <v>2.5</v>
       </c>
-      <c r="B7" s="65">
+      <c r="B7" s="66">
         <v>1.4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="64">
+      <c r="A8" s="65">
         <v>3.0</v>
       </c>
-      <c r="B8" s="65">
+      <c r="B8" s="66">
         <v>1.5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="64">
+      <c r="A9" s="65">
         <v>3.5</v>
       </c>
-      <c r="B9" s="65">
+      <c r="B9" s="66">
         <v>1.6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="64">
+      <c r="A10" s="65">
         <v>4.0</v>
       </c>
-      <c r="B10" s="65">
+      <c r="B10" s="66">
         <v>1.7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="64">
+      <c r="A11" s="65">
         <v>4.5</v>
       </c>
-      <c r="B11" s="65">
+      <c r="B11" s="66">
         <v>1.8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="64">
+      <c r="A12" s="65">
         <v>5.0</v>
       </c>
-      <c r="B12" s="65">
+      <c r="B12" s="66">
         <v>1.8</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="64">
+      <c r="A13" s="65">
         <v>5.5</v>
       </c>
-      <c r="B13" s="65">
+      <c r="B13" s="66">
         <v>1.9</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="64">
+      <c r="A14" s="65">
         <v>6.0</v>
       </c>
-      <c r="B14" s="65">
+      <c r="B14" s="66">
         <v>2.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="64">
+      <c r="A15" s="65">
         <v>6.5</v>
       </c>
-      <c r="B15" s="65">
+      <c r="B15" s="66">
         <v>2.1</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="64">
+      <c r="A16" s="65">
         <v>7.0</v>
       </c>
-      <c r="B16" s="65">
+      <c r="B16" s="66">
         <v>2.2</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="64">
+      <c r="A17" s="65">
         <v>7.5</v>
       </c>
-      <c r="B17" s="65">
+      <c r="B17" s="66">
         <v>2.3</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="64">
+      <c r="A18" s="65">
         <v>8.0</v>
       </c>
-      <c r="B18" s="65">
+      <c r="B18" s="66">
         <v>2.3</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="64">
+      <c r="A19" s="65">
         <v>8.5</v>
       </c>
-      <c r="B19" s="65">
+      <c r="B19" s="66">
         <v>2.4</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="64">
+      <c r="A20" s="65">
         <v>9.0</v>
       </c>
-      <c r="B20" s="65">
+      <c r="B20" s="66">
         <v>2.5</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="64">
+      <c r="A21" s="65">
         <v>9.5</v>
       </c>
-      <c r="B21" s="65">
+      <c r="B21" s="66">
         <v>2.6</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="64">
+      <c r="A22" s="65">
         <v>10.0</v>
       </c>
-      <c r="B22" s="65">
+      <c r="B22" s="66">
         <v>2.7</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="64">
+      <c r="A23" s="65">
         <v>10.5</v>
       </c>
-      <c r="B23" s="65">
+      <c r="B23" s="66">
         <v>2.8</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="64">
+      <c r="A24" s="65">
         <v>11.0</v>
       </c>
-      <c r="B24" s="65">
+      <c r="B24" s="66">
         <v>2.8</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="64">
+      <c r="A25" s="65">
         <v>11.5</v>
       </c>
-      <c r="B25" s="65">
+      <c r="B25" s="66">
         <v>2.9</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="64">
+      <c r="A26" s="65">
         <v>12.0</v>
       </c>
-      <c r="B26" s="65">
+      <c r="B26" s="66">
         <v>3.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="64">
+      <c r="A27" s="65">
         <v>12.5</v>
       </c>
-      <c r="B27" s="65">
+      <c r="B27" s="66">
         <v>3.1</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="64">
+      <c r="A28" s="65">
         <v>13.0</v>
       </c>
-      <c r="B28" s="65">
+      <c r="B28" s="66">
         <v>3.2</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="64">
+      <c r="A29" s="65">
         <v>13.5</v>
       </c>
-      <c r="B29" s="65">
+      <c r="B29" s="66">
         <v>3.3</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="64">
+      <c r="A30" s="65">
         <v>14.0</v>
       </c>
-      <c r="B30" s="65">
+      <c r="B30" s="66">
         <v>3.3</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="64">
+      <c r="A31" s="65">
         <v>14.5</v>
       </c>
-      <c r="B31" s="65">
+      <c r="B31" s="66">
         <v>3.4</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="64">
+      <c r="A32" s="65">
         <v>15.0</v>
       </c>
-      <c r="B32" s="65">
+      <c r="B32" s="66">
         <v>3.5</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="64">
+      <c r="A33" s="65">
         <v>15.5</v>
       </c>
-      <c r="B33" s="65">
+      <c r="B33" s="66">
         <v>3.6</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="64">
+      <c r="A34" s="65">
         <v>16.0</v>
       </c>
-      <c r="B34" s="65">
+      <c r="B34" s="66">
         <v>3.7</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="64">
+      <c r="A35" s="65">
         <v>16.5</v>
       </c>
-      <c r="B35" s="65">
+      <c r="B35" s="66">
         <v>3.8</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="64">
+      <c r="A36" s="65">
         <v>17.0</v>
       </c>
-      <c r="B36" s="65">
+      <c r="B36" s="66">
         <v>3.8</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="64">
+      <c r="A37" s="65">
         <v>17.5</v>
       </c>
-      <c r="B37" s="65">
+      <c r="B37" s="66">
         <v>3.9</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="64">
+      <c r="A38" s="65">
         <v>18.0</v>
       </c>
-      <c r="B38" s="65">
+      <c r="B38" s="66">
         <v>4.0</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="64">
+      <c r="A39" s="65">
         <v>18.5</v>
       </c>
-      <c r="B39" s="65">
+      <c r="B39" s="66">
         <v>4.1</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="64">
+      <c r="A40" s="65">
         <v>19.0</v>
       </c>
-      <c r="B40" s="65">
+      <c r="B40" s="66">
         <v>4.3</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="64">
+      <c r="A41" s="65">
         <v>19.5</v>
       </c>
-      <c r="B41" s="65">
+      <c r="B41" s="66">
         <v>4.4</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="64">
+      <c r="A42" s="65">
         <v>20.0</v>
       </c>
-      <c r="B42" s="65">
+      <c r="B42" s="66">
         <v>4.5</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="64">
+      <c r="A43" s="65">
         <v>20.5</v>
       </c>
-      <c r="B43" s="65">
+      <c r="B43" s="66">
         <v>4.6</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="64">
+      <c r="A44" s="65">
         <v>21.0</v>
       </c>
-      <c r="B44" s="65">
+      <c r="B44" s="66">
         <v>4.8</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="64">
+      <c r="A45" s="65">
         <v>21.5</v>
       </c>
-      <c r="B45" s="65">
+      <c r="B45" s="66">
         <v>4.9</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="64">
+      <c r="A46" s="65">
         <v>22.0</v>
       </c>
-      <c r="B46" s="65">
+      <c r="B46" s="66">
         <v>5.0</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="64">
+      <c r="A47" s="65">
         <v>22.5</v>
       </c>
-      <c r="B47" s="65">
+      <c r="B47" s="66">
         <v>5.1</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="64">
+      <c r="A48" s="65">
         <v>23.0</v>
       </c>
-      <c r="B48" s="65">
+      <c r="B48" s="66">
         <v>5.3</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="64">
+      <c r="A49" s="65">
         <v>23.5</v>
       </c>
-      <c r="B49" s="65">
+      <c r="B49" s="66">
         <v>5.4</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="64">
+      <c r="A50" s="65">
         <v>24.0</v>
       </c>
-      <c r="B50" s="65">
+      <c r="B50" s="66">
         <v>5.5</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="64">
+      <c r="A51" s="65">
         <v>24.5</v>
       </c>
-      <c r="B51" s="65">
+      <c r="B51" s="66">
         <v>5.6</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="64">
+      <c r="A52" s="65">
         <v>25.0</v>
       </c>
-      <c r="B52" s="65">
+      <c r="B52" s="66">
         <v>5.8</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="64">
+      <c r="A53" s="65">
         <v>25.5</v>
       </c>
-      <c r="B53" s="65">
+      <c r="B53" s="66">
         <v>5.9</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="64">
+      <c r="A54" s="65">
         <v>26.0</v>
       </c>
-      <c r="B54" s="65">
+      <c r="B54" s="66">
         <v>6.0</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="64">
+      <c r="A55" s="65">
         <v>26.5</v>
       </c>
-      <c r="B55" s="65">
+      <c r="B55" s="66">
         <v>6.1</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="64">
+      <c r="A56" s="65">
         <v>27.0</v>
       </c>
-      <c r="B56" s="65">
+      <c r="B56" s="66">
         <v>6.3</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="64">
+      <c r="A57" s="65">
         <v>27.5</v>
       </c>
-      <c r="B57" s="65">
+      <c r="B57" s="66">
         <v>6.4</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="64">
+      <c r="A58" s="65">
         <v>28.0</v>
       </c>
-      <c r="B58" s="65">
+      <c r="B58" s="66">
         <v>6.5</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="64">
+      <c r="A59" s="65">
         <v>28.5</v>
       </c>
-      <c r="B59" s="65">
+      <c r="B59" s="66">
         <v>6.6</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="64">
+      <c r="A60" s="65">
         <v>29.0</v>
       </c>
-      <c r="B60" s="65">
+      <c r="B60" s="66">
         <v>6.8</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="64">
+      <c r="A61" s="65">
         <v>29.5</v>
       </c>
-      <c r="B61" s="65">
+      <c r="B61" s="66">
         <v>6.9</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="64">
+      <c r="A62" s="65">
         <v>30.0</v>
       </c>
-      <c r="B62" s="65">
+      <c r="B62" s="66">
         <v>7.0</v>
       </c>
     </row>
@@ -9842,61 +9840,61 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="66" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="69"/>
+      <c r="A1" s="67" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="70"/>
     </row>
     <row r="2">
-      <c r="A2" s="70"/>
-      <c r="B2" s="71" t="s">
+      <c r="A2" s="71"/>
+      <c r="B2" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="72" t="s">
-        <v>96</v>
-      </c>
-      <c r="E2" s="73" t="s">
+      <c r="D2" s="73" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="74" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="74" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="75">
+      <c r="A3" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="76">
         <v>4.0</v>
       </c>
-      <c r="C3" s="75">
+      <c r="C3" s="76">
         <v>3.0</v>
       </c>
-      <c r="D3" s="75">
+      <c r="D3" s="76">
         <v>2.0</v>
       </c>
-      <c r="E3" s="75">
+      <c r="E3" s="76">
         <v>0.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="74"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
+      <c r="A4" s="75"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
     </row>
     <row r="5">
-      <c r="A5" s="74"/>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
+      <c r="A5" s="75"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>